<commit_message>
Initial commit of adjusted tumor BCA
</commit_message>
<xml_diff>
--- a/Western_blot/BCA/unknown_data_subset.xlsx
+++ b/Western_blot/BCA/unknown_data_subset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nunley17/Documents/Lab/Experiments/Experiments_2024/MYCN-IDH1-In-Vivo-experiments-03-22-2024/Western_blot/BCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{109D2D94-98C9-0B4D-81A4-71BD5D5E56D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B8B452-59B7-1C43-92BB-EEE9D180172F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33800" yWindow="2780" windowWidth="26200" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Replicate</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>IDH1-M2-1-E</t>
-  </si>
-  <si>
-    <t>IDH1-M2-1-F</t>
   </si>
 </sst>
 </file>
@@ -432,15 +429,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,11 +480,8 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -529,9 +523,6 @@
       </c>
       <c r="N2">
         <v>0.24909999999999999</v>
-      </c>
-      <c r="O2">
-        <v>0.46419999000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'IDH1-M2-1-F' back to WB Rep1
</commit_message>
<xml_diff>
--- a/Western_blot/BCA/unknown_data_subset.xlsx
+++ b/Western_blot/BCA/unknown_data_subset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nunley17/Documents/Lab/Experiments/Experiments_2024/MYCN-IDH1-In-Vivo-experiments-03-22-2024/Western_blot/BCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B8B452-59B7-1C43-92BB-EEE9D180172F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3351F9-6969-804D-9D68-A1A5E26A354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33800" yWindow="2780" windowWidth="26200" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Replicate</t>
   </si>
@@ -429,15 +429,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +480,11 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -523,6 +526,9 @@
       </c>
       <c r="N2">
         <v>0.24909999999999999</v>
+      </c>
+      <c r="O2">
+        <v>0.62029999499999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed last sample in BCA rep1
</commit_message>
<xml_diff>
--- a/Western_blot/BCA/unknown_data_subset.xlsx
+++ b/Western_blot/BCA/unknown_data_subset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nunley17/Documents/Lab/Experiments/Experiments_2024/MYCN-IDH1-In-Vivo-experiments-03-22-2024/Western_blot/BCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3351F9-6969-804D-9D68-A1A5E26A354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EE2A53-F594-084C-A767-DEEF26F96504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33800" yWindow="2780" windowWidth="26200" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Replicate</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>IDH1-M2-1-E</t>
+  </si>
+  <si>
+    <t>IDH1-M2-1-F</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -481,7 +484,7 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -528,7 +531,7 @@
         <v>0.24909999999999999</v>
       </c>
       <c r="O2">
-        <v>0.62029999499999999</v>
+        <v>0.46419999000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>